<commit_message>
feat(vendors): update excel receipt template
</commit_message>
<xml_diff>
--- a/src/main/resources/abrechnung_template.xlsx
+++ b/src/main/resources/abrechnung_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Abrechnung" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Verkäufer Nummer:</t>
   </si>
   <si>
-    <t>Übersicht über alle verkaufen Artikel</t>
+    <t>Übersicht über alle verkauften Artikel</t>
   </si>
 </sst>
 </file>
@@ -88,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -112,7 +112,30 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF103FA6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF103FA6"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -141,15 +164,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFCFDDFB"/>
       </left>
@@ -175,11 +189,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -194,20 +219,28 @@
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -249,7 +282,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -546,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,16 +604,17 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -621,26 +661,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -655,7 +696,7 @@
     <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>